<commit_message>
send email functionality, some test cases
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andoni_Aguirre_Arang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andoni_Aguirre_Arang\Desktop\UiPath\CalculateClientHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226C6E20-DD87-48D3-9D9C-4EC0EC9124EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B71BBCA-96A7-4AD5-BE25-010D5A5B1C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25860" yWindow="3810" windowWidth="21585" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>MaxRetryNumberDispatcher</t>
+  </si>
+  <si>
+    <t>EmailRecipients</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1677,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2848,7 +2851,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2906,8 +2909,28 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>